<commit_message>
fix lôi bảng xem trước
</commit_message>
<xml_diff>
--- a/userList.xlsx
+++ b/userList.xlsx
@@ -13,23 +13,22 @@
   </bookViews>
   <sheets>
     <sheet name="list" sheetId="1" r:id="rId1"/>
+    <sheet name="ds" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">list!$A$1:$I$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ds!$A$1:$G$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">list!$A$1:$I$72</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="329">
   <si>
     <t>TT</t>
   </si>
   <si>
-    <t>Chức vụ</t>
-  </si>
-  <si>
     <t>Hồ Ngọc Cường</t>
   </si>
   <si>
@@ -201,12 +200,6 @@
     <t>Phạm Thị Ánh Tuyết</t>
   </si>
   <si>
-    <t>TTCM</t>
-  </si>
-  <si>
-    <t>TPCM</t>
-  </si>
-  <si>
     <t>Phan  Bảo Quốc</t>
   </si>
   <si>
@@ -234,15 +227,9 @@
     <t>Đặng Hồng Liên</t>
   </si>
   <si>
-    <t>Giáo viên</t>
-  </si>
-  <si>
     <t>Toán</t>
   </si>
   <si>
-    <t>Vật lý</t>
-  </si>
-  <si>
     <t>CNCN</t>
   </si>
   <si>
@@ -267,15 +254,6 @@
     <t>Địa lý</t>
   </si>
   <si>
-    <t>GDCD</t>
-  </si>
-  <si>
-    <t>Thể dục</t>
-  </si>
-  <si>
-    <t>GDQP</t>
-  </si>
-  <si>
     <t>Tiếng Anh</t>
   </si>
   <si>
@@ -964,6 +942,75 @@
   </si>
   <si>
     <t>bp</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>Tổ Vật lí -CNCN</t>
+  </si>
+  <si>
+    <t>Tổ Địa lí - Lịch sử</t>
+  </si>
+  <si>
+    <t>Thể dục - QP</t>
+  </si>
+  <si>
+    <t>Thể dục - QP - Tin học</t>
+  </si>
+  <si>
+    <t>KTGD&amp;PL</t>
+  </si>
+  <si>
+    <t>Tổ Ngữ văn - KTGD&amp;PL</t>
+  </si>
+  <si>
+    <t>Tổ Hoá học - Sinh học - CNNN</t>
+  </si>
+  <si>
+    <t>Tổ Tiếng Anh</t>
+  </si>
+  <si>
+    <t>Tổ Toán</t>
+  </si>
+  <si>
+    <t>Vật lí</t>
+  </si>
+  <si>
+    <t>Lê Thị Quỳnh Trang</t>
+  </si>
+  <si>
+    <t>Bùi Thị Thuỷ</t>
+  </si>
+  <si>
+    <t>Hà Thị Mỹ Trang</t>
+  </si>
+  <si>
+    <t>Học và tên</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Đơn vị</t>
+  </si>
+  <si>
+    <t>Môn dạy</t>
+  </si>
+  <si>
+    <t>SĐT</t>
+  </si>
+  <si>
+    <t>htmtrangdk2@gmail.com</t>
+  </si>
+  <si>
+    <t>2sGbRFM2m0fnzZp4LYNdXc6VMbm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lequynhtrang2012@gmail.com </t>
+  </si>
+  <si>
+    <t>vY6Lbf2XuxOCx8qUtBXMQJVAe0u1</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1144,6 +1191,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1168,13 +1233,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1200,6 +1265,66 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="8067675" y="2476500"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="https://mail.google.com/mail/u/0/images/cleardot.gif"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4210050" y="571500"/>
           <a:ext cx="9525" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1509,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1647,7 @@
     <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="10" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="32"/>
@@ -1535,2006 +1660,3708 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <f t="shared" ref="A2:A33" si="0">ROW()-1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>299</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
-        <f>ROW()-1</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="13" t="s">
+      <c r="C3" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="I3" s="30"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="I2" s="29"/>
-    </row>
-    <row r="3" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <f>ROW()-1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="I3" s="29"/>
-    </row>
-    <row r="4" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <f>ROW()-1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="I4" s="29"/>
+      <c r="H4" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>70</v>
+        <v>308</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I5" s="30"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>59</v>
+        <v>308</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>70</v>
+        <v>308</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>70</v>
+        <v>308</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>141</v>
+        <v>264</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>70</v>
+        <v>308</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="I9" s="30"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>60</v>
+        <v>308</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="I10" s="30"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>70</v>
+        <v>308</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>219</v>
+        <v>74</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>184</v>
       </c>
       <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>283</v>
+        <v>238</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>213</v>
+        <v>131</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="I12" s="30"/>
+      <c r="H12" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>282</v>
+        <v>243</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>70</v>
+        <v>313</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>216</v>
+        <v>72</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>176</v>
       </c>
       <c r="I13" s="30"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>284</v>
+        <v>241</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>70</v>
+        <v>313</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>218</v>
+        <v>72</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>70</v>
+        <v>313</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>60</v>
+        <v>313</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>70</v>
+        <v>313</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>252</v>
+        <v>173</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>70</v>
+        <v>313</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="I18" s="30"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>250</v>
+      <c r="B19" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>239</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>70</v>
+        <v>313</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="I19" s="30"/>
+        <v>174</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>181</v>
+        <v>129</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>70</v>
+        <v>313</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="I20" s="30"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>247</v>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>237</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>177</v>
+        <v>130</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>59</v>
+        <v>313</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="I21" s="31" t="s">
-        <v>220</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
-        <f>ROW()-1</f>
+      <c r="A22" s="13">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>307</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>204</v>
+      <c r="B22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>144</v>
       </c>
       <c r="I22" s="30"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>194</v>
+        <v>128</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>70</v>
+        <v>313</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="I23" s="30"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>272</v>
+        <v>134</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>312</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>79</v>
+        <v>311</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="I24" s="30"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>189</v>
+        <v>133</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>60</v>
+        <v>294</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>312</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>79</v>
+        <v>311</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>191</v>
+        <v>136</v>
       </c>
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>312</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>79</v>
+        <v>311</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="I26" s="30"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
-        <f>ROW()-1</f>
+      <c r="A27" s="13">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>307</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>205</v>
+      <c r="B27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>141</v>
       </c>
       <c r="I27" s="30"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
-        <f>ROW()-1</f>
+      <c r="A28" s="13">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>307</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="H28" s="25" t="s">
-        <v>203</v>
+      <c r="B28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>138</v>
       </c>
       <c r="I28" s="30"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>116</v>
+        <v>256</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>312</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="I29" s="30"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>266</v>
+        <v>109</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>312</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I30" s="30"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>264</v>
+        <v>107</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>312</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="I31" s="30"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>312</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="I32" s="30"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>22</v>
+        <v>317</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>261</v>
+        <v>328</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>115</v>
+        <v>327</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>59</v>
+        <v>294</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>312</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" s="19" t="s">
-        <v>150</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H33" s="19"/>
       <c r="I33" s="30"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" ref="A34:A65" si="1">ROW()-1</f>
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>70</v>
+        <v>314</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="I34" s="30"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>244</v>
+        <v>283</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>70</v>
+        <v>314</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="I35" s="30"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>245</v>
+        <v>278</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>138</v>
+        <v>89</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>70</v>
+        <v>314</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H36" s="19" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="I36" s="30"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>242</v>
+        <v>285</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>60</v>
+        <v>314</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H37" s="19" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
       <c r="I37" s="30"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>243</v>
+        <v>280</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>136</v>
+        <v>91</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>70</v>
+        <v>314</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>153</v>
+        <v>99</v>
       </c>
       <c r="I38" s="30"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>70</v>
+        <v>314</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="I39" s="30"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>70</v>
+        <v>314</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="I40" s="30"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>59</v>
+        <v>314</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I41" s="30"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>104</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="C42" s="18"/>
+      <c r="D42" s="14"/>
       <c r="E42" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H42" s="19" t="s">
-        <v>112</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="H42" s="19"/>
       <c r="I42" s="30"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>288</v>
+        <v>219</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>107</v>
+        <v>162</v>
       </c>
       <c r="I43" s="30"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>289</v>
+        <v>224</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="I44" s="30"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>98</v>
+        <v>149</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>60</v>
+        <v>315</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
       <c r="I45" s="30"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>290</v>
+        <v>225</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="I46" s="30"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>95</v>
+        <v>156</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="I47" s="30"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>258</v>
+        <v>217</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="I48" s="30"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>94</v>
+        <v>164</v>
       </c>
       <c r="I49" s="30"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>87</v>
+        <v>155</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>60</v>
+        <v>315</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H50" s="19" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
       <c r="I50" s="30"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>257</v>
+        <v>218</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>89</v>
+        <v>151</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H51" s="19" t="s">
-        <v>90</v>
+        <v>161</v>
       </c>
       <c r="I51" s="31" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>227</v>
+      <c r="B52" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>220</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="I52" s="30"/>
+        <v>163</v>
+      </c>
+      <c r="I52" s="31" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>70</v>
+        <v>307</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H53" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="I53" s="30"/>
+        <v>68</v>
+      </c>
+      <c r="H53" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="I53" s="29"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>60</v>
+        <v>307</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H54" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="I54" s="30"/>
+        <v>68</v>
+      </c>
+      <c r="H54" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="I54" s="29"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>166</v>
+        <v>117</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>70</v>
+        <v>307</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H55" s="19" t="s">
-        <v>176</v>
+        <v>316</v>
+      </c>
+      <c r="H55" s="21" t="s">
+        <v>118</v>
       </c>
       <c r="I55" s="30"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>6</v>
+        <v>319</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>231</v>
+        <v>326</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>164</v>
+        <v>325</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>70</v>
+        <v>307</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H56" s="19" t="s">
-        <v>174</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="H56" s="21"/>
       <c r="I56" s="30"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>158</v>
+        <v>113</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>70</v>
+        <v>307</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H57" s="19" t="s">
-        <v>168</v>
+        <v>316</v>
+      </c>
+      <c r="H57" s="21" t="s">
+        <v>114</v>
       </c>
       <c r="I57" s="30"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>70</v>
+        <v>307</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H58" s="19" t="s">
-        <v>172</v>
+        <v>316</v>
+      </c>
+      <c r="H58" s="21" t="s">
+        <v>116</v>
       </c>
       <c r="I58" s="30"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>70</v>
+        <v>307</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H59" s="19" t="s">
-        <v>173</v>
+        <v>316</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="I59" s="30"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="13">
-        <f>ROW()-1</f>
+      <c r="A60" s="1">
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="B60" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C60" s="23" t="s">
+      <c r="B60" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="D60" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>302</v>
+      <c r="D60" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E60" s="28" t="s">
+        <v>294</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>70</v>
+        <v>307</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H60" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="I60" s="31" t="s">
-        <v>220</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I60" s="30"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B61" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>228</v>
+      <c r="B61" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>230</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>70</v>
+        <v>307</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H61" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="I61" s="31" t="s">
-        <v>220</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="H61" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="I61" s="30"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>310</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>82</v>
+        <v>309</v>
       </c>
       <c r="H62" s="20" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I62" s="30"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>59</v>
+        <v>294</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>310</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>82</v>
+        <v>309</v>
       </c>
       <c r="H63" s="20" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I63" s="30"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>237</v>
+        <v>274</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>125</v>
+        <v>202</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>310</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H64" s="21" t="s">
-        <v>126</v>
+        <v>309</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="I64" s="30"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>235</v>
+        <v>276</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>60</v>
+        <v>294</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>310</v>
       </c>
       <c r="G65" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H65" s="21" t="s">
-        <v>122</v>
+        <v>309</v>
+      </c>
+      <c r="H65" s="20" t="s">
+        <v>210</v>
       </c>
       <c r="I65" s="30"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" ref="A66:A74" si="2">ROW()-1</f>
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>310</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H66" s="21" t="s">
-        <v>124</v>
+        <v>71</v>
+      </c>
+      <c r="H66" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="I66" s="30"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>310</v>
       </c>
       <c r="G67" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H67" s="21" t="s">
-        <v>130</v>
+        <v>71</v>
+      </c>
+      <c r="H67" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="I67" s="30"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <f>ROW()-1</f>
+      <c r="A68" s="13">
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="B68" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C68" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="D68" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="E68" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="F68" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H68" s="21" t="s">
-        <v>120</v>
+      <c r="B68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H68" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="I68" s="30"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>70</v>
+        <v>294</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>310</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H69" s="21" t="s">
-        <v>128</v>
+        <v>71</v>
+      </c>
+      <c r="H69" s="19" t="s">
+        <v>80</v>
       </c>
       <c r="I69" s="30"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>295</v>
+      <c r="B70" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="23" t="s">
+        <v>249</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>294</v>
+        <v>81</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="G70" s="13"/>
+        <v>294</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="H70" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="I70" s="30"/>
+        <v>82</v>
+      </c>
+      <c r="I70" s="31" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="E71" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="F71" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G71" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="H71" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="I71" s="30"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="13">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E72" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G72" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="H72" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="I72" s="30"/>
+    </row>
+    <row r="73" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="13">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G73" s="13"/>
+      <c r="H73" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="I73" s="30"/>
+    </row>
+    <row r="74" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="13">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G74" s="13"/>
+      <c r="H74" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="I74" s="30"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G75" s="4"/>
+      <c r="H75" s="9"/>
+    </row>
+    <row r="81" spans="7:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G81" s="5"/>
+      <c r="H81" s="11"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I72">
+    <sortState ref="A2:I71">
+      <sortCondition ref="F1:F71"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0" right="0" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G79"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="32"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <f t="shared" ref="A2:A33" si="0">ROW()-1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="G2" s="30"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="30"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="G10" s="30"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="G11" s="30"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="30"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="G14" s="30"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="G15" s="30"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="G16" s="30"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="G17" s="30"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="G18" s="30"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="33">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" s="30"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="30"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G23" s="30"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="C71" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="E71" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="F71" s="2" t="s">
+      <c r="E24" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G24" s="30"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="30"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" s="30"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" s="30"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="30"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="G29" s="30"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="G30" s="30"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="30"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="G32" s="30"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="35"/>
+      <c r="G33" s="37"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <f t="shared" ref="A34:A65" si="1">ROW()-1</f>
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G34" s="30"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" s="30"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G36" s="30"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="G37" s="30"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" s="30"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G39" s="30"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G40" s="30"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G41" s="30"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="33">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="C42" s="34"/>
+      <c r="D42" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" s="35"/>
+      <c r="G42" s="37"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="13">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="G43" s="30"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="13">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="G44" s="30"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="13">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="G45" s="30"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="13">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="G46" s="30"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="13">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="G47" s="30"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="G48" s="30"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="13">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="G49" s="30"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="13">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="G50" s="30"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="33">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F51" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="G51" s="36" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="33">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="E52" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="G52" s="36" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G53" s="29"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="13">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="G54" s="29"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="13">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="G55" s="30"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="33">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="C56" s="34"/>
+      <c r="D56" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="F56" s="38"/>
+      <c r="G56" s="37"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="13">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G57" s="30"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="13">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G58" s="30"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="13">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G59" s="30"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B60" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G60" s="30"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="13">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="G61" s="30"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="13">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D62" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="G71" s="13"/>
-      <c r="H71" s="19" t="s">
-        <v>305</v>
-      </c>
-      <c r="I71" s="30"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G72" s="4"/>
-      <c r="H72" s="9"/>
-    </row>
-    <row r="78" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="G78" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H78" s="11"/>
+      <c r="E62" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="F62" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="G62" s="30"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="13">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="G63" s="30"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="13">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="G64" s="30"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="13">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="F65" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="G65" s="30"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="13">
+        <f t="shared" ref="A66:A72" si="2">ROW()-1</f>
+        <v>65</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G66" s="30"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="13">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G67" s="30"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="13">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G68" s="30"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="13">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G69" s="30"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="33">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D70" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="E70" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="G70" s="36" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="13">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="F71" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="G71" s="30"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="13">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="F72" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="G72" s="30"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E73" s="4"/>
+      <c r="F73" s="9"/>
+    </row>
+    <row r="79" spans="1:7" s="32" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A79"/>
+      <c r="B79"/>
+      <c r="C79" s="6"/>
+      <c r="D79"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I71"/>
+  <autoFilter ref="A1:G72">
+    <sortState ref="A2:I71">
+      <sortCondition ref="D1:D71"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0" right="0" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Thể dục => Giáo dục thể chất
</commit_message>
<xml_diff>
--- a/userList.xlsx
+++ b/userList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="330">
   <si>
     <t>TT</t>
   </si>
@@ -1011,6 +1011,9 @@
   </si>
   <si>
     <t>vY6Lbf2XuxOCx8qUtBXMQJVAe0u1</t>
+  </si>
+  <si>
+    <t>thuyc3camlo@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1636,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2813,7 +2816,9 @@
         <v>318</v>
       </c>
       <c r="C42" s="18"/>
-      <c r="D42" s="14"/>
+      <c r="D42" s="14" t="s">
+        <v>329</v>
+      </c>
       <c r="E42" s="18" t="s">
         <v>294</v>
       </c>

</xml_diff>

<commit_message>
fix modal đăng ký gia diện mobile
</commit_message>
<xml_diff>
--- a/userList.xlsx
+++ b/userList.xlsx
@@ -19,12 +19,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ds!$A$1:$G$72</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">list!$A$1:$I$72</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="333">
   <si>
     <t>TT</t>
   </si>
@@ -698,9 +698,6 @@
     <t>lfHdhWRgNdhf3lzHPGTqOk1ns4u1</t>
   </si>
   <si>
-    <t>25PDf0wrp7VUj5oahi9YEDUPJm92</t>
-  </si>
-  <si>
     <t>U4HdGg54f8hzYFaw3jde3M5Z3wp2</t>
   </si>
   <si>
@@ -740,9 +737,6 @@
     <t>k03nB9QmJUQFpWXsgItXHwHzgZ62</t>
   </si>
   <si>
-    <t>dSrLphLSoxSJKyuniUWQVikVPFd2</t>
-  </si>
-  <si>
     <t>gTtcayYQsCcY9cWfHg2OrprIWF02</t>
   </si>
   <si>
@@ -1014,12 +1008,27 @@
   </si>
   <si>
     <t>thuyc3camlo@gmail.com</t>
+  </si>
+  <si>
+    <t>SlKqnFdc42cmT2NJ8iYys47BWE53</t>
+  </si>
+  <si>
+    <t>thanhtienclv@gmail.com</t>
+  </si>
+  <si>
+    <t>jTo0slHWwYNjfRXQe12ctW5fuLu2</t>
+  </si>
+  <si>
+    <t>nguyendanhdatqt@gmail.com</t>
+  </si>
+  <si>
+    <t>nOc0Enyqimf1mftg1hJ27N2P4sM2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1640,7 +1649,7 @@
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,28 +1672,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>293</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1702,7 +1711,7 @@
         <v>194</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>77</v>
@@ -1730,7 +1739,7 @@
         <v>198</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>78</v>
@@ -1758,7 +1767,7 @@
         <v>199</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>78</v>
@@ -1780,16 +1789,16 @@
         <v>6</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>192</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>75</v>
@@ -1808,16 +1817,16 @@
         <v>11</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>188</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>75</v>
@@ -1836,16 +1845,16 @@
         <v>41</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>190</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>75</v>
@@ -1864,16 +1873,16 @@
         <v>55</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>186</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>74</v>
@@ -1892,16 +1901,16 @@
         <v>56</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>74</v>
@@ -1920,16 +1929,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>181</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>74</v>
@@ -1948,16 +1957,16 @@
         <v>52</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>182</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>74</v>
@@ -1976,16 +1985,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>238</v>
+        <v>332</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>131</v>
+        <v>331</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>70</v>
@@ -2004,16 +2013,16 @@
         <v>46</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>171</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>72</v>
@@ -2032,16 +2041,16 @@
         <v>8</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>72</v>
@@ -2060,16 +2069,16 @@
         <v>16</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>172</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>72</v>
@@ -2088,16 +2097,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>72</v>
@@ -2116,16 +2125,16 @@
         <v>27</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>170</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>72</v>
@@ -2144,16 +2153,16 @@
         <v>15</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>173</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>72</v>
@@ -2172,16 +2181,16 @@
         <v>45</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>169</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>72</v>
@@ -2202,16 +2211,16 @@
         <v>35</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>129</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>69</v>
@@ -2230,16 +2239,16 @@
         <v>36</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>130</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>69</v>
@@ -2258,16 +2267,16 @@
         <v>17</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>127</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>69</v>
@@ -2286,16 +2295,16 @@
         <v>30</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>128</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>69</v>
@@ -2314,19 +2323,19 @@
         <v>53</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>134</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>137</v>
@@ -2342,19 +2351,19 @@
         <v>64</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>133</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H25" s="19" t="s">
         <v>136</v>
@@ -2370,19 +2379,19 @@
         <v>22</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>132</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H26" s="19" t="s">
         <v>135</v>
@@ -2398,16 +2407,16 @@
         <v>39</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>108</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>73</v>
@@ -2426,16 +2435,16 @@
         <v>62</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>73</v>
@@ -2454,16 +2463,16 @@
         <v>38</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>73</v>
@@ -2482,16 +2491,16 @@
         <v>34</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>73</v>
@@ -2510,16 +2519,16 @@
         <v>21</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>107</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>73</v>
@@ -2538,16 +2547,16 @@
         <v>63</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>110</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>73</v>
@@ -2563,19 +2572,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>73</v>
@@ -2592,16 +2601,16 @@
         <v>7</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>95</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>76</v>
@@ -2620,16 +2629,16 @@
         <v>66</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>94</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>76</v>
@@ -2648,16 +2657,16 @@
         <v>31</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>89</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>76</v>
@@ -2676,16 +2685,16 @@
         <v>43</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>96</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>76</v>
@@ -2704,16 +2713,16 @@
         <v>3</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>76</v>
@@ -2732,16 +2741,16 @@
         <v>65</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>92</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>76</v>
@@ -2760,16 +2769,16 @@
         <v>14</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>90</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>76</v>
@@ -2788,16 +2797,16 @@
         <v>23</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>93</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>76</v>
@@ -2813,17 +2822,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="C42" s="18"/>
+        <v>316</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>328</v>
+      </c>
       <c r="D42" s="14" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>67</v>
@@ -2846,10 +2857,10 @@
         <v>152</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>67</v>
@@ -2868,16 +2879,16 @@
         <v>50</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>224</v>
+        <v>330</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>157</v>
+        <v>329</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G44" s="13" t="s">
         <v>67</v>
@@ -2902,10 +2913,10 @@
         <v>149</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G45" s="13" t="s">
         <v>67</v>
@@ -2924,16 +2935,16 @@
         <v>105</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>158</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>67</v>
@@ -2958,10 +2969,10 @@
         <v>156</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>67</v>
@@ -2986,10 +2997,10 @@
         <v>150</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>67</v>
@@ -3014,10 +3025,10 @@
         <v>154</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G49" s="13" t="s">
         <v>67</v>
@@ -3042,10 +3053,10 @@
         <v>155</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>67</v>
@@ -3070,10 +3081,10 @@
         <v>151</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>67</v>
@@ -3100,10 +3111,10 @@
         <v>153</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G52" s="13" t="s">
         <v>67</v>
@@ -3124,16 +3135,16 @@
         <v>20</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>125</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G53" s="13" t="s">
         <v>68</v>
@@ -3152,16 +3163,16 @@
         <v>37</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D54" s="14" t="s">
         <v>123</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G54" s="13" t="s">
         <v>68</v>
@@ -3180,19 +3191,19 @@
         <v>19</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D55" s="14" t="s">
         <v>117</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H55" s="21" t="s">
         <v>118</v>
@@ -3205,22 +3216,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H56" s="21"/>
       <c r="I56" s="30"/>
@@ -3234,19 +3245,19 @@
         <v>12</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D57" s="14" t="s">
         <v>113</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H57" s="21" t="s">
         <v>114</v>
@@ -3262,19 +3273,19 @@
         <v>106</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D58" s="14" t="s">
         <v>115</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H58" s="21" t="s">
         <v>116</v>
@@ -3290,19 +3301,19 @@
         <v>42</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D59" s="14" t="s">
         <v>121</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H59" s="21" t="s">
         <v>122</v>
@@ -3318,19 +3329,19 @@
         <v>18</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D60" s="17" t="s">
         <v>111</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H60" s="21" t="s">
         <v>112</v>
@@ -3346,19 +3357,19 @@
         <v>26</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D61" s="14" t="s">
         <v>119</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H61" s="21" t="s">
         <v>120</v>
@@ -3374,19 +3385,19 @@
         <v>49</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D62" s="14" t="s">
         <v>201</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H62" s="20" t="s">
         <v>211</v>
@@ -3402,19 +3413,19 @@
         <v>28</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D63" s="14" t="s">
         <v>205</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H63" s="20" t="s">
         <v>209</v>
@@ -3430,19 +3441,19 @@
         <v>25</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D64" s="14" t="s">
         <v>202</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H64" s="20" t="s">
         <v>208</v>
@@ -3458,19 +3469,19 @@
         <v>33</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>203</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G65" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H65" s="20" t="s">
         <v>210</v>
@@ -3486,16 +3497,16 @@
         <v>47</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>87</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>71</v>
@@ -3514,16 +3525,16 @@
         <v>61</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>83</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>71</v>
@@ -3542,16 +3553,16 @@
         <v>24</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D68" s="14" t="s">
         <v>85</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>71</v>
@@ -3570,16 +3581,16 @@
         <v>32</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D69" s="14" t="s">
         <v>79</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>71</v>
@@ -3598,16 +3609,16 @@
         <v>48</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D70" s="14" t="s">
         <v>81</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>71</v>
@@ -3628,19 +3639,19 @@
         <v>44</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D71" s="14" t="s">
         <v>204</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H71" s="20" t="s">
         <v>207</v>
@@ -3656,19 +3667,19 @@
         <v>40</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D72" s="14" t="s">
         <v>200</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H72" s="20" t="s">
         <v>206</v>
@@ -3681,23 +3692,23 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G73" s="13"/>
       <c r="H73" s="19" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I73" s="30"/>
     </row>
@@ -3707,23 +3718,23 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G74" s="13"/>
       <c r="H74" s="19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I74" s="30"/>
     </row>
@@ -3741,9 +3752,12 @@
       <sortCondition ref="F1:F71"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="D44" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0" right="0" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3773,19 +3787,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>322</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>324</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>212</v>
@@ -3869,7 +3883,7 @@
         <v>192</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>75</v>
@@ -3891,7 +3905,7 @@
         <v>188</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>75</v>
@@ -3913,7 +3927,7 @@
         <v>190</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>75</v>
@@ -3935,7 +3949,7 @@
         <v>186</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>74</v>
@@ -3954,10 +3968,10 @@
         <v>56</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>74</v>
@@ -3979,7 +3993,7 @@
         <v>181</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>74</v>
@@ -4001,7 +4015,7 @@
         <v>182</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>74</v>
@@ -4023,7 +4037,7 @@
         <v>131</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>70</v>
@@ -4045,7 +4059,7 @@
         <v>171</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>72</v>
@@ -4064,10 +4078,10 @@
         <v>8</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>72</v>
@@ -4089,7 +4103,7 @@
         <v>172</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>72</v>
@@ -4108,10 +4122,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>72</v>
@@ -4133,7 +4147,7 @@
         <v>170</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>72</v>
@@ -4155,7 +4169,7 @@
         <v>173</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>72</v>
@@ -4177,7 +4191,7 @@
         <v>169</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E19" s="33" t="s">
         <v>72</v>
@@ -4201,7 +4215,7 @@
         <v>129</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>69</v>
@@ -4223,7 +4237,7 @@
         <v>130</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>69</v>
@@ -4245,7 +4259,7 @@
         <v>127</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>69</v>
@@ -4267,7 +4281,7 @@
         <v>128</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>69</v>
@@ -4289,10 +4303,10 @@
         <v>134</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F24" s="19" t="s">
         <v>137</v>
@@ -4311,10 +4325,10 @@
         <v>133</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F25" s="19" t="s">
         <v>136</v>
@@ -4333,10 +4347,10 @@
         <v>132</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>135</v>
@@ -4355,7 +4369,7 @@
         <v>108</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>73</v>
@@ -4374,10 +4388,10 @@
         <v>62</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>73</v>
@@ -4396,10 +4410,10 @@
         <v>38</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>73</v>
@@ -4421,7 +4435,7 @@
         <v>109</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>73</v>
@@ -4443,7 +4457,7 @@
         <v>107</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>73</v>
@@ -4465,7 +4479,7 @@
         <v>110</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>73</v>
@@ -4481,11 +4495,11 @@
         <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C33" s="34"/>
       <c r="D33" s="33" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E33" s="33" t="s">
         <v>73</v>
@@ -4505,7 +4519,7 @@
         <v>95</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>76</v>
@@ -4527,7 +4541,7 @@
         <v>94</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>76</v>
@@ -4549,7 +4563,7 @@
         <v>89</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>76</v>
@@ -4571,7 +4585,7 @@
         <v>96</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>76</v>
@@ -4593,7 +4607,7 @@
         <v>91</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>76</v>
@@ -4615,7 +4629,7 @@
         <v>92</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>76</v>
@@ -4637,7 +4651,7 @@
         <v>90</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>76</v>
@@ -4659,7 +4673,7 @@
         <v>93</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E41" s="13" t="s">
         <v>76</v>
@@ -4675,11 +4689,11 @@
         <v>41</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C42" s="34"/>
       <c r="D42" s="22" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E42" s="33" t="s">
         <v>67</v>
@@ -4699,7 +4713,7 @@
         <v>152</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>67</v>
@@ -4721,7 +4735,7 @@
         <v>157</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>67</v>
@@ -4743,7 +4757,7 @@
         <v>149</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>67</v>
@@ -4765,7 +4779,7 @@
         <v>158</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E46" s="13" t="s">
         <v>67</v>
@@ -4787,7 +4801,7 @@
         <v>156</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>67</v>
@@ -4809,7 +4823,7 @@
         <v>150</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>67</v>
@@ -4831,7 +4845,7 @@
         <v>154</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>67</v>
@@ -4853,7 +4867,7 @@
         <v>155</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>67</v>
@@ -4875,7 +4889,7 @@
         <v>151</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E51" s="33" t="s">
         <v>67</v>
@@ -4899,7 +4913,7 @@
         <v>153</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E52" s="33" t="s">
         <v>67</v>
@@ -4923,7 +4937,7 @@
         <v>125</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>68</v>
@@ -4945,7 +4959,7 @@
         <v>123</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E54" s="13" t="s">
         <v>68</v>
@@ -4967,10 +4981,10 @@
         <v>117</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F55" s="21" t="s">
         <v>118</v>
@@ -4983,14 +4997,14 @@
         <v>55</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C56" s="34"/>
       <c r="D56" s="22" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F56" s="38"/>
       <c r="G56" s="37"/>
@@ -5007,10 +5021,10 @@
         <v>113</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F57" s="21" t="s">
         <v>114</v>
@@ -5029,10 +5043,10 @@
         <v>115</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F58" s="21" t="s">
         <v>116</v>
@@ -5051,10 +5065,10 @@
         <v>121</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F59" s="21" t="s">
         <v>122</v>
@@ -5073,10 +5087,10 @@
         <v>111</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F60" s="21" t="s">
         <v>112</v>
@@ -5095,10 +5109,10 @@
         <v>119</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F61" s="21" t="s">
         <v>120</v>
@@ -5117,10 +5131,10 @@
         <v>201</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F62" s="20" t="s">
         <v>211</v>
@@ -5139,10 +5153,10 @@
         <v>205</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F63" s="20" t="s">
         <v>209</v>
@@ -5161,10 +5175,10 @@
         <v>202</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F64" s="20" t="s">
         <v>208</v>
@@ -5183,10 +5197,10 @@
         <v>203</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F65" s="20" t="s">
         <v>210</v>
@@ -5205,7 +5219,7 @@
         <v>87</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E66" s="13" t="s">
         <v>71</v>
@@ -5227,7 +5241,7 @@
         <v>83</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E67" s="13" t="s">
         <v>71</v>
@@ -5249,7 +5263,7 @@
         <v>85</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E68" s="13" t="s">
         <v>71</v>
@@ -5271,7 +5285,7 @@
         <v>79</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E69" s="13" t="s">
         <v>71</v>
@@ -5293,7 +5307,7 @@
         <v>81</v>
       </c>
       <c r="D70" s="33" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E70" s="33" t="s">
         <v>71</v>
@@ -5317,10 +5331,10 @@
         <v>204</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F71" s="20" t="s">
         <v>207</v>
@@ -5339,10 +5353,10 @@
         <v>200</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F72" s="20" t="s">
         <v>206</v>

</xml_diff>